<commit_message>
All the work we did with Naja today. Set up (perhaps?) final data, ran ANOVA tests.
</commit_message>
<xml_diff>
--- a/conditionsR.xlsx
+++ b/conditionsR.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tania\OneDrive\Skrivebord\Thesis_Experiments\Outputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tania\OneDrive\Skrivebord\Thesis-R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9A3F68D-562C-441F-9E24-49BAAA899E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E08C738-987B-4CC8-90AD-D0F40802BFF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{6C178E21-7D7B-4816-989B-C3F83C4E56A7}"/>
   </bookViews>
@@ -1020,9 +1020,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D81D423A-6C74-4832-B956-835A43D9B43C}">
   <dimension ref="A1:N97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.90625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>